<commit_message>
compressor compressibility factor add
</commit_message>
<xml_diff>
--- a/amplify/backend/function/h2auxcalculator/src/lib/compressor_specs_example.xlsx
+++ b/amplify/backend/function/h2auxcalculator/src/lib/compressor_specs_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://greencathydrogenltd-my.sharepoint.com/personal/pavel_culik_gchydrogen_co_uk/Documents/Documents/GitHub/GCH/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Culik\Documents\GitHub\H2AuxInvestTest\amplify\backend\function\h2auxcalculator\src\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9FF8648F-9E67-4DF3-BD53-240169E76E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5C9BE9C-1B30-4AD1-A73F-B58C621F6676}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A51A0DE-CBC4-4607-9F12-CD9FF77A990F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9A77C2FC-938C-4A28-9002-CDFA8E88A87C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A77C2FC-938C-4A28-9002-CDFA8E88A87C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -121,9 +119,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -161,7 +159,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -267,7 +265,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -409,7 +407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -420,15 +418,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -439,11 +437,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2">
+        <v>0.82</v>
+      </c>
       <c r="C2" s="2">
         <v>0.79</v>
       </c>
@@ -451,7 +451,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -465,12 +465,12 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>0.77</v>
+        <v>0.78</v>
       </c>
       <c r="C4" s="2">
         <v>0.79</v>
@@ -479,7 +479,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>

</xml_diff>